<commit_message>
Interay blockbax data analysis
</commit_message>
<xml_diff>
--- a/Temperature compensation optimisation/Interay/141421/SB_141421_Interay_val_3_cleaned.xlsx
+++ b/Temperature compensation optimisation/Interay/141421/SB_141421_Interay_val_3_cleaned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://althennl-my.sharepoint.com/personal/m_brummelhuis_althen_nl/Documents/Documenten/GitHub/Althen/Temperature compensation optimisation/Interay/141421/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_BB73F8E72470074B70EB6672E93161BA83D1047F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C26DE38-081D-4563-9F9F-B13D3B403D74}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_BB73F8E72470074B70EB6672E93161BA83D1047F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B28E799E-64AE-4BE1-BAC8-E68932695738}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,13 +71,13 @@
     <t>Interval</t>
   </si>
   <si>
-    <t>Yw/o offset</t>
-  </si>
-  <si>
     <t>ref angle</t>
   </si>
   <si>
     <t>Offset (20C)</t>
+  </si>
+  <si>
+    <t>Y w/o offset</t>
   </si>
 </sst>
 </file>
@@ -85,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -118,7 +118,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -458,18 +458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L573"/>
+  <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N181" sqref="N181"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,13 +501,13 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44620.833703703705</v>
       </c>
@@ -546,7 +546,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44620.837175925924</v>
       </c>
@@ -585,7 +585,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44620.840648148151</v>
       </c>
@@ -624,7 +624,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44620.84412037037</v>
       </c>
@@ -663,7 +663,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44620.847592592596</v>
       </c>
@@ -702,7 +702,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44620.851064814815</v>
       </c>
@@ -741,7 +741,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44620.854537037034</v>
       </c>
@@ -780,7 +780,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44620.85800925926</v>
       </c>
@@ -819,7 +819,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44620.861481481479</v>
       </c>
@@ -858,7 +858,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44620.864953703705</v>
       </c>
@@ -897,7 +897,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44620.868425925924</v>
       </c>
@@ -936,7 +936,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44620.871898148151</v>
       </c>
@@ -975,7 +975,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44620.87537037037</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44620.878842592596</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44620.882314814815</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44620.885787037034</v>
       </c>
@@ -1131,7 +1131,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44620.88925925926</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44620.892731481479</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44620.896203703705</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44620.899675925924</v>
       </c>
@@ -1287,7 +1287,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44620.903148148151</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44620.90662037037</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44620.910092592596</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44620.913564814815</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44620.917037037034</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>1.0470999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44621.00037037037</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44621.003842592596</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44621.007314814815</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44621.010787037034</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44621.01425925926</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44621.017731481479</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44621.021203703705</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44621.024675925924</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44621.028148148151</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44621.03162037037</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44621.035092592596</v>
       </c>
@@ -1922,7 +1922,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44621.038564814815</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44621.042037037034</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44621.04550925926</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44621.048981481479</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44621.052453703705</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44621.055925925924</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44621.059398148151</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44621.06287037037</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44621.066342592596</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44621.069814814815</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44621.073287037034</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44621.07675925926</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44621.080231481479</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44621.083703703705</v>
       </c>
@@ -2482,7 +2482,7 @@
         <v>1.0391999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44621.167037037034</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44621.17050925926</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44621.173981481479</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="55" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44621.177453703705</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44621.180925925924</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44621.184398148151</v>
       </c>
@@ -2716,7 +2716,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44621.18787037037</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44621.191342592596</v>
       </c>
@@ -2794,7 +2794,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44621.194814814815</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44621.198287037034</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44621.20175925926</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44621.205231481479</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44621.208703703705</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44621.212175925924</v>
       </c>
@@ -3028,7 +3028,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44621.215648148151</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44621.21912037037</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44621.222592592596</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44621.226064814815</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44621.229537037034</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44621.23300925926</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44621.236481481479</v>
       </c>
@@ -3301,7 +3301,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44621.239953703705</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44621.243425925924</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44621.246898148151</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44621.25037037037</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>1.028</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44621.333703703705</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44621.337175925924</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44621.340648148151</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44621.34412037037</v>
       </c>
@@ -3613,7 +3613,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44621.347592592596</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44621.351064814815</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44621.354537037034</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44621.35800925926</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44621.361481481479</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44621.364953703705</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44621.368425925924</v>
       </c>
@@ -3886,7 +3886,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44621.371898148151</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>44621.37537037037</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>44621.378842592596</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>44621.382314814815</v>
       </c>
@@ -4042,7 +4042,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>44621.385787037034</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>44621.38925925926</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>44621.392731481479</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>44621.396203703705</v>
       </c>
@@ -4198,7 +4198,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>44621.399675925924</v>
       </c>
@@ -4237,7 +4237,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>44621.403148148151</v>
       </c>
@@ -4276,7 +4276,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>44621.40662037037</v>
       </c>
@@ -4315,7 +4315,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>44621.410092592596</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>44621.413564814815</v>
       </c>
@@ -4393,7 +4393,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>44621.417037037034</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>1.0194000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>44621.50037037037</v>
       </c>
@@ -4471,7 +4471,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>44621.503842592596</v>
       </c>
@@ -4510,7 +4510,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>44621.507314814815</v>
       </c>
@@ -4549,7 +4549,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>44621.510787037034</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>44621.51425925926</v>
       </c>
@@ -4627,7 +4627,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>44621.517731481479</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>44621.521203703705</v>
       </c>
@@ -4705,7 +4705,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>44621.524675925924</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>44621.528148148151</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>44621.53162037037</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>44621.535092592596</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>44621.538564814815</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>44621.542037037034</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>44621.54550925926</v>
       </c>
@@ -4978,7 +4978,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>44621.548981481479</v>
       </c>
@@ -5017,7 +5017,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>44621.552453703705</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>44621.555925925924</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>44621.559398148151</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>44621.56287037037</v>
       </c>
@@ -5173,7 +5173,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>44621.566342592596</v>
       </c>
@@ -5212,7 +5212,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>44621.569814814815</v>
       </c>
@@ -5251,7 +5251,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>44621.573287037034</v>
       </c>
@@ -5290,7 +5290,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>44621.57675925926</v>
       </c>
@@ -5329,7 +5329,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>44621.580231481479</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>44621.583703703705</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>1.0162</v>
       </c>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>44621.667037037034</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>44621.67050925926</v>
       </c>
@@ -5485,7 +5485,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>44621.673981481479</v>
       </c>
@@ -5524,7 +5524,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>44621.677453703705</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>44621.680925925924</v>
       </c>
@@ -5602,7 +5602,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>44621.684398148151</v>
       </c>
@@ -5641,7 +5641,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>44621.68787037037</v>
       </c>
@@ -5680,7 +5680,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="134" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>44621.691342592596</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="135" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>44621.694814814815</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="136" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>44621.698287037034</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="137" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>44621.70175925926</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="138" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>44621.705231481479</v>
       </c>
@@ -5875,7 +5875,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="139" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>44621.708703703705</v>
       </c>
@@ -5914,7 +5914,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="140" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>44621.712175925924</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>44621.715648148151</v>
       </c>
@@ -5992,7 +5992,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="142" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>44621.71912037037</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="143" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>44621.722592592596</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="144" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>44621.726064814815</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="145" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>44621.729537037034</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="146" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>44621.73300925926</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="147" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>44621.736481481479</v>
       </c>
@@ -6226,7 +6226,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>44621.739953703705</v>
       </c>
@@ -6265,7 +6265,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="149" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>44621.743425925924</v>
       </c>
@@ -6304,7 +6304,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="150" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>44621.746898148151</v>
       </c>
@@ -6343,7 +6343,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="151" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>44621.75037037037</v>
       </c>
@@ -6382,7 +6382,7 @@
         <v>1.0178</v>
       </c>
     </row>
-    <row r="152" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>44621.833703703705</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="153" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>44621.837175925924</v>
       </c>
@@ -6460,7 +6460,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>44621.840648148151</v>
       </c>
@@ -6499,7 +6499,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="155" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>44621.84412037037</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="156" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>44621.847592592596</v>
       </c>
@@ -6577,7 +6577,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>44621.851064814815</v>
       </c>
@@ -6616,7 +6616,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="158" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>44621.854537037034</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="159" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>44621.85800925926</v>
       </c>
@@ -6694,7 +6694,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="160" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>44621.861481481479</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="161" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>44621.864953703705</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="162" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>44621.868425925924</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="163" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>44621.871898148151</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>44621.87537037037</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="165" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>44621.878842592596</v>
       </c>
@@ -6928,7 +6928,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="166" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>44621.882314814815</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>44621.885787037034</v>
       </c>
@@ -7006,7 +7006,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>44621.88925925926</v>
       </c>
@@ -7045,7 +7045,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>44621.892731481479</v>
       </c>
@@ -7084,7 +7084,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>44621.896203703705</v>
       </c>
@@ -7123,7 +7123,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>44621.899675925924</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="172" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>44621.903148148151</v>
       </c>
@@ -7201,7 +7201,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="173" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>44621.90662037037</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>44621.910092592596</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="175" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>44621.913564814815</v>
       </c>
@@ -7318,7 +7318,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="176" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>44621.917037037034</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>1.0154000000000001</v>
       </c>
     </row>
-    <row r="177" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>44622.00037037037</v>
       </c>
@@ -7396,7 +7396,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="178" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>44622.003842592596</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>44622.007314814815</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="180" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>44622.010787037034</v>
       </c>
@@ -7513,7 +7513,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="181" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>44622.01425925926</v>
       </c>
@@ -7552,7 +7552,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>44622.017731481479</v>
       </c>
@@ -7591,7 +7591,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>44622.021203703705</v>
       </c>
@@ -7630,7 +7630,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="184" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>44622.024675925924</v>
       </c>
@@ -7669,7 +7669,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="185" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>44622.028148148151</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="186" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>44622.03162037037</v>
       </c>
@@ -7747,7 +7747,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="187" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>44622.035092592596</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="188" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>44622.038564814815</v>
       </c>
@@ -7825,7 +7825,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>44622.042037037034</v>
       </c>
@@ -7864,7 +7864,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="190" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44622.04550925926</v>
       </c>
@@ -7903,7 +7903,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="191" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44622.048981481479</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="192" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44622.052453703705</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="193" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44622.055925925924</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="194" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44622.059398148151</v>
       </c>
@@ -8059,7 +8059,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="195" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44622.06287037037</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44622.066342592596</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="197" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44622.069814814815</v>
       </c>
@@ -8176,7 +8176,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="198" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44622.073287037034</v>
       </c>
@@ -8215,7 +8215,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="199" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44622.07675925926</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="200" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44622.080231481479</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="201" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44622.083703703705</v>
       </c>
@@ -8332,72 +8332,6 @@
         <v>1.0112000000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="204" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="205" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="206" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="207" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="208" spans="1:12" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:J201" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8419,7 +8353,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>